<commit_message>
Corrected SQL bug and code cleanup
Found that the SQL bug was that sizing days were being added to the
table.  Rewrote code to extract only the data from weather period run

Also, major cleanup of the processSQL to reduce bloat and improve
readability
</commit_message>
<xml_diff>
--- a/Install/Simulation_Output_Settings.xlsx
+++ b/Install/Simulation_Output_Settings.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>electricityHeating</t>
   </si>
@@ -739,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -760,12 +760,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +806,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed timestep bug and refactored uncertainty code
fixed bug where timestep not extracted properly in process_SQL because
it's called "zone timestep" in the SQL but is requested by asking for
"timestep" .  Also did a little cleanup on uncertainty code
</commit_message>
<xml_diff>
--- a/Install/Simulation_Output_Settings.xlsx
+++ b/Install/Simulation_Output_Settings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TotalEnergy" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>electricityHeating</t>
   </si>
@@ -739,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -763,26 +763,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -793,7 +773,7 @@
           <x14:formula1>
             <xm:f>Sources!$A$2:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A24</xm:sqref>
+          <xm:sqref>A2:A25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -803,10 +783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -828,15 +808,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -849,13 +821,13 @@
           <x14:formula1>
             <xm:f>Sources!$E$2:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B30</xm:sqref>
+          <xm:sqref>B2:B24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sources!$D$2:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A30</xm:sqref>
+          <xm:sqref>A2:A24</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -868,7 +840,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Combined LHS_Gen.rb and Morris.rb
Combined LHS_Gen.rb and Morris.rb into a single file LHS_Morris.rb to
reduce duplicate code in the two files and have only one version of
cdf_inverse to edit/maintain
</commit_message>
<xml_diff>
--- a/Install/Simulation_Output_Settings.xlsx
+++ b/Install/Simulation_Output_Settings.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14640" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TotalEnergy" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="69">
   <si>
     <t>electricityHeating</t>
   </si>
@@ -762,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -814,10 +814,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -839,30 +839,14 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -900,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Got BC_setup.rb and BC.rb working except ...
BC_setup.rb and BC.rb working again.  Had to update code to use the new
vertical format for the meter outputs process_simulation_SQLx.
Posteriosr are generated and plotted. Still don't have the code working
to create a calibrated model.
</commit_message>
<xml_diff>
--- a/Install/Simulation_Output_Settings.xlsx
+++ b/Install/Simulation_Output_Settings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14640" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TotalEnergy" sheetId="1" r:id="rId1"/>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -884,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>